<commit_message>
rerun elprop and test score
Pulled elprop from student level data to deal with missing; re-ran test scores using the all scores sample with one score obs per student
</commit_message>
<xml_diff>
--- a/out/xls/factoranalysis/to latex/VA Mechinsims - Survey Regs_updated.xlsx
+++ b/out/xls/factoranalysis/to latex/VA Mechinsims - Survey Regs_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Dropbox\Davis\Research Projects\Ed Lab GSR\caschls\out\xls\factoranalysis\to latex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC87337E-A959-42BD-ADFB-FD619983BFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A35250-8E4F-4D36-AB9E-9922ED2DB493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9570" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="112">
   <si>
     <t>Value Added Variables</t>
   </si>
@@ -255,9 +255,6 @@
     <t>370</t>
   </si>
   <si>
-    <t>-0.09</t>
-  </si>
-  <si>
     <t>-0.03</t>
   </si>
   <si>
@@ -294,36 +291,21 @@
     <t>898</t>
   </si>
   <si>
-    <t>889</t>
-  </si>
-  <si>
-    <t>888</t>
-  </si>
-  <si>
     <t>0.11***</t>
   </si>
   <si>
     <t>0.06*</t>
   </si>
   <si>
-    <t>-0.07*</t>
-  </si>
-  <si>
     <t>-0.07**</t>
   </si>
   <si>
-    <t>-0.06*</t>
-  </si>
-  <si>
     <t>(0.03)</t>
   </si>
   <si>
     <t>0.12***</t>
   </si>
   <si>
-    <t>0.07*</t>
-  </si>
-  <si>
     <t>-0.10***</t>
   </si>
   <si>
@@ -333,18 +315,9 @@
     <t>0.09***</t>
   </si>
   <si>
-    <t>0.06**</t>
-  </si>
-  <si>
     <t>0.08**</t>
   </si>
   <si>
-    <t>386</t>
-  </si>
-  <si>
-    <t>380</t>
-  </si>
-  <si>
     <t>0.16**</t>
   </si>
   <si>
@@ -354,19 +327,49 @@
     <t>-0.10</t>
   </si>
   <si>
-    <t>0.14**</t>
-  </si>
-  <si>
-    <t>281</t>
-  </si>
-  <si>
     <t>0.10*</t>
   </si>
   <si>
-    <t>367</t>
-  </si>
-  <si>
-    <t>366</t>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>0.14***</t>
+  </si>
+  <si>
+    <t>0.11*</t>
+  </si>
+  <si>
+    <t>-0.11*</t>
+  </si>
+  <si>
+    <t>0.13**</t>
+  </si>
+  <si>
+    <t>0.09*</t>
+  </si>
+  <si>
+    <t>-0.02</t>
+  </si>
+  <si>
+    <t>0.10**</t>
+  </si>
+  <si>
+    <t>-0.08**</t>
+  </si>
+  <si>
+    <t>-0.01</t>
+  </si>
+  <si>
+    <t>-0.12***</t>
+  </si>
+  <si>
+    <t>-0.11***</t>
+  </si>
+  <si>
+    <t>909</t>
+  </si>
+  <si>
+    <t>897</t>
   </si>
 </sst>
 </file>
@@ -760,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R34" sqref="R33:R34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -871,10 +874,10 @@
         <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
@@ -950,46 +953,46 @@
         <v>30</v>
       </c>
       <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
         <v>78</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>78</v>
       </c>
-      <c r="D7" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" t="s">
-        <v>79</v>
-      </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -1100,46 +1103,46 @@
         <v>30</v>
       </c>
       <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E10" t="s">
-        <v>81</v>
-      </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.35">
@@ -1238,46 +1241,46 @@
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
         <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
         <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L13" t="s">
         <v>72</v>
       </c>
       <c r="M13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="N13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.35">
@@ -1624,7 +1627,7 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.35">
@@ -1635,54 +1638,54 @@
         <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>65</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>34</v>
@@ -1723,46 +1726,46 @@
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.35">
@@ -1770,57 +1773,57 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>18</v>
@@ -1841,7 +1844,7 @@
         <v>34</v>
       </c>
       <c r="K29" s="5" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="L29" s="5" t="s">
         <v>34</v>
@@ -1861,46 +1864,46 @@
         <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.35">
@@ -1908,46 +1911,46 @@
         <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -1955,7 +1958,7 @@
         <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>65</v>
@@ -1999,51 +2002,51 @@
         <v>30</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="E33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>109</v>
-      </c>
       <c r="I33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="K33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="M33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>110</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.35">
@@ -2051,43 +2054,43 @@
         <v>22</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="F36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>57</v>
@@ -2101,7 +2104,7 @@
         <v>56</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>56</v>
@@ -2142,46 +2145,46 @@
         <v>23</v>
       </c>
       <c r="B38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="D38" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -2233,90 +2236,90 @@
         <v>45</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>20</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="K41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="L41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="N41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="O41" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.35">
@@ -2324,46 +2327,46 @@
         <v>30</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="K42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="N42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="O42" s="7" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>